<commit_message>
added nba teams and script to create folders and parse out the games for each team of that season
</commit_message>
<xml_diff>
--- a/nba/NBATeams.xlsx
+++ b/nba/NBATeams.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>GSW</t>
   </si>
@@ -33,103 +33,64 @@
     <t>https://www.basketball-reference.com/teams/CLE/2016.html</t>
   </si>
   <si>
-    <t>2015-16</t>
-  </si>
-  <si>
     <t>LAL</t>
   </si>
   <si>
-    <t>2014-15</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/GSW/2015.html</t>
   </si>
   <si>
     <t>https://www.basketball-reference.com/teams/GSW/2017.html</t>
   </si>
   <si>
-    <t>2016-17</t>
-  </si>
-  <si>
-    <t>Bulls</t>
-  </si>
-  <si>
-    <t>1995-96</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/CHI/1996.html</t>
   </si>
   <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>1985-86</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/BOS/1986.html</t>
   </si>
   <si>
-    <t>1986-87</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/LAL/1987.html</t>
   </si>
   <si>
-    <t>1990-91</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/CHI/1991.html</t>
   </si>
   <si>
-    <t>1996-97</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/CHI/1997.html</t>
   </si>
   <si>
-    <t>Spurs</t>
-  </si>
-  <si>
-    <t>2013-14</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/SAS/2014.html</t>
   </si>
   <si>
-    <t>2007-08</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/BOS/2008.html</t>
   </si>
   <si>
-    <t>2008-09</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/LAL/2009.html</t>
   </si>
   <si>
     <t>https://www.basketball-reference.com/teams/LAL/2002.html</t>
   </si>
   <si>
-    <t>2001-02</t>
-  </si>
-  <si>
     <t>DAL</t>
   </si>
   <si>
-    <t>2010-11</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/DAL/2011.html</t>
   </si>
   <si>
-    <t>2012-13</t>
-  </si>
-  <si>
     <t>https://www.basketball-reference.com/teams/MIA/2013.html</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>MIA</t>
   </si>
 </sst>
 </file>
@@ -493,7 +454,7 @@
   <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,19 +479,19 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+      <c r="B2" s="1">
+        <v>2017</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2016</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -538,134 +499,134 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2002</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+      <c r="B5" s="1">
+        <v>2015</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1996</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1986</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1987</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1991</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1997</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2014</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2008</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2009</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2011</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2013</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">

</xml_diff>